<commit_message>
Fixed column names to match predict_personality
</commit_message>
<xml_diff>
--- a/data/word_pool.xlsx
+++ b/data/word_pool.xlsx
@@ -14,30 +14,30 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="648" uniqueCount="622">
-  <si>
-    <t>artista</t>
-  </si>
-  <si>
-    <t>diva</t>
-  </si>
-  <si>
-    <t>oa</t>
-  </si>
-  <si>
-    <t>wildcard</t>
-  </si>
-  <si>
-    <t>achiever</t>
-  </si>
-  <si>
-    <t>emo</t>
-  </si>
-  <si>
-    <t>gamer</t>
-  </si>
-  <si>
-    <t>softie</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="648" uniqueCount="621">
+  <si>
+    <t>Artista</t>
+  </si>
+  <si>
+    <t>Diva</t>
+  </si>
+  <si>
+    <t>OA</t>
+  </si>
+  <si>
+    <t>Wildcard</t>
+  </si>
+  <si>
+    <t>Achiever</t>
+  </si>
+  <si>
+    <t>EMO</t>
+  </si>
+  <si>
+    <t>Gamer</t>
+  </si>
+  <si>
+    <t>Softie</t>
   </si>
   <si>
     <t xml:space="preserve">Aesthetic  </t>
@@ -1871,9 +1871,6 @@
   </si>
   <si>
     <t>King</t>
-  </si>
-  <si>
-    <t>Achiever</t>
   </si>
   <si>
     <t xml:space="preserve">Frownie  </t>
@@ -4352,13 +4349,13 @@
         <v>618</v>
       </c>
       <c r="E81" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="F81" s="2" t="s">
         <v>619</v>
       </c>
-      <c r="F81" s="2" t="s">
+      <c r="G81" s="2" t="s">
         <v>620</v>
-      </c>
-      <c r="G81" s="2" t="s">
-        <v>621</v>
       </c>
       <c r="H81" s="2" t="s">
         <v>465</v>

</xml_diff>